<commit_message>
Add Conditional Effects -- WIP
</commit_message>
<xml_diff>
--- a/Resources/details.xlsx
+++ b/Resources/details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b52fca1a386bca4b/Documents/Creative/Programming/Python/Caverna/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alastairc\Documents\Creative\Caverna\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="271" documentId="102_{121A5001-816A-4708-9BBF-EAA567F93A7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9D1F18B9-3F2F-4016-9D2D-297C1F9BD40A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5893883-84DA-4EC4-9CF0-CC3E10C62578}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5010" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{985A88D9-ACD6-4D50-8968-6DB430F624CA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{985A88D9-ACD6-4D50-8968-6DB430F624CA}"/>
   </bookViews>
   <sheets>
     <sheet name="action cards" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="764">
   <si>
     <t>name</t>
   </si>
@@ -2328,6 +2328,9 @@
   </si>
   <si>
     <t>waiting on change food conversion rate</t>
+  </si>
+  <si>
+    <t>waiting on conversion</t>
   </si>
 </sst>
 </file>
@@ -3015,7 +3018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15391F36-646A-4811-8FB5-C926ED9F13BD}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D46" sqref="D46:D51"/>
     </sheetView>
   </sheetViews>
@@ -4124,8 +4127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03460E6A-234E-4B76-A2F7-FDC0B540496D}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4740,7 +4743,9 @@
         <v>143</v>
       </c>
       <c r="H27" s="10"/>
-      <c r="I27" s="11"/>
+      <c r="I27" s="11" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -4857,7 +4862,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>176</v>
       </c>
@@ -4880,7 +4885,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>177</v>
       </c>
@@ -4906,7 +4911,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>178</v>
       </c>
@@ -4926,7 +4931,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>179</v>
       </c>
@@ -4946,7 +4951,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>180</v>
       </c>
@@ -4966,7 +4971,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>191</v>
       </c>
@@ -4986,7 +4991,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>192</v>
       </c>
@@ -5006,7 +5011,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>193</v>
       </c>
@@ -5025,8 +5030,11 @@
       <c r="G40" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>194</v>
       </c>
@@ -5046,7 +5054,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>195</v>
       </c>
@@ -5066,7 +5074,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>196</v>
       </c>
@@ -5086,7 +5094,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>220</v>
       </c>
@@ -5106,7 +5114,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>221</v>
       </c>
@@ -5126,7 +5134,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>222</v>
       </c>
@@ -5146,7 +5154,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>223</v>
       </c>
@@ -5166,7 +5174,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>224</v>
       </c>

</xml_diff>

<commit_message>
add base Game runner actions
</commit_message>
<xml_diff>
--- a/Resources/details.xlsx
+++ b/Resources/details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alastairc\Documents\Creative\Caverna\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b52fca1a386bca4b/Documents/Creative/Programming/Python/Caverna/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2F82B9-6E2C-4068-AA04-9F654C7652B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="114_{E01527BB-0BB8-414C-97A2-6D3BF0239F55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{23D8E027-1C59-47C1-9CF8-A55D8659A361}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{985A88D9-ACD6-4D50-8968-6DB430F624CA}"/>
+    <workbookView xWindow="28680" yWindow="-5010" windowWidth="29040" windowHeight="15840" xr2:uid="{985A88D9-ACD6-4D50-8968-6DB430F624CA}"/>
   </bookViews>
   <sheets>
     <sheet name="action cards" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="764">
   <si>
     <t>name</t>
   </si>
@@ -959,9 +960,6 @@
     <t>breeding phase</t>
   </si>
   <si>
-    <t>gain 1 animal for every animal for which you have 1 pair</t>
-  </si>
-  <si>
     <t>per each animal and each dog</t>
   </si>
   <si>
@@ -2319,6 +2317,21 @@
   </si>
   <si>
     <t>waiting on action effects</t>
+  </si>
+  <si>
+    <t>7C3 possible harvest phases</t>
+  </si>
+  <si>
+    <t>3! Possible level 1 card draws</t>
+  </si>
+  <si>
+    <t>3! Possible level 4 card draws</t>
+  </si>
+  <si>
+    <t>3! Possible level 5 card draws</t>
+  </si>
+  <si>
+    <t>2! Possible level 2 card draws</t>
   </si>
 </sst>
 </file>
@@ -2377,14 +2390,39 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="18">
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF7030A0"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2399,65 +2437,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDDFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0C1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2597,27 +2582,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2680,11 +2644,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A3CC4776-1BB1-47A4-A2A9-F8775571405D}" name="Table3" displayName="Table3" ref="A1:B53" totalsRowShown="0" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A3CC4776-1BB1-47A4-A2A9-F8775571405D}" name="Table3" displayName="Table3" ref="A1:B53" totalsRowShown="0" dataDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A1:B53" xr:uid="{A4EB2E2A-BCC8-4327-8FD8-7B69602999D4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{59D50046-B7D9-4882-AFEC-FF0243C53E0B}" name="action value function output" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{13ED629A-1E3C-4AD1-844A-C53BC838B743}" name="value" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{59D50046-B7D9-4882-AFEC-FF0243C53E0B}" name="action value function output" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{13ED629A-1E3C-4AD1-844A-C53BC838B743}" name="value" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3000,8 +2964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15391F36-646A-4811-8FB5-C926ED9F13BD}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3021,7 +2985,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3045,7 +3009,7 @@
         <v>48</v>
       </c>
       <c r="J1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3295,7 +3259,7 @@
         <v>-1</v>
       </c>
       <c r="D11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E11" t="s">
         <v>65</v>
@@ -3400,7 +3364,7 @@
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>75</v>
@@ -3672,7 +3636,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B26">
         <v>24</v>
@@ -3906,7 +3870,7 @@
         <v>50</v>
       </c>
       <c r="G35" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>283</v>
@@ -3988,9 +3952,6 @@
       <c r="D44" t="s">
         <v>305</v>
       </c>
-      <c r="E44" t="s">
-        <v>306</v>
-      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -4002,6 +3963,12 @@
       <c r="D46" t="s">
         <v>295</v>
       </c>
+      <c r="E46" t="s">
+        <v>759</v>
+      </c>
+      <c r="F46">
+        <v>35</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47">
@@ -4010,6 +3977,13 @@
       <c r="D47" t="s">
         <v>107</v>
       </c>
+      <c r="E47" t="s">
+        <v>760</v>
+      </c>
+      <c r="F47">
+        <f>FACT(3)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48">
@@ -4018,32 +3992,57 @@
       <c r="D48" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>763</v>
+      </c>
+      <c r="F48">
+        <f>FACT(2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>3</v>
       </c>
       <c r="D49" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>761</v>
+      </c>
+      <c r="F49">
+        <f t="shared" ref="F49:F50" si="0">FACT(3)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>4</v>
       </c>
       <c r="D50" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>762</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>5</v>
       </c>
       <c r="D51" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f>PRODUCT(F46:F50)</f>
+        <v>15120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>299</v>
       </c>
@@ -4054,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>301</v>
       </c>
@@ -4062,7 +4061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>302</v>
       </c>
@@ -4075,40 +4074,40 @@
     <sortCondition ref="C31"/>
   </sortState>
   <conditionalFormatting sqref="D2:E35">
-    <cfRule type="containsText" dxfId="10" priority="5" stopIfTrue="1" operator="containsText" text="take accumulated">
+    <cfRule type="containsText" dxfId="13" priority="5" stopIfTrue="1" operator="containsText" text="take accumulated">
       <formula>NOT(ISERROR(SEARCH("take accumulated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="expedition">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="expedition">
       <formula>NOT(ISERROR(SEARCH("expedition",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="7" stopIfTrue="1" operator="containsText" text="baby dwarf">
+    <cfRule type="containsText" dxfId="11" priority="7" stopIfTrue="1" operator="containsText" text="baby dwarf">
       <formula>NOT(ISERROR(SEARCH("baby dwarf",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="furnish">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="furnish">
       <formula>NOT(ISERROR(SEARCH("furnish",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="place a">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="place a">
       <formula>NOT(ISERROR(SEARCH("place a",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="receive">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="receive">
       <formula>NOT(ISERROR(SEARCH("receive",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text="pay">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="pay">
       <formula>NOT(ISERROR(SEARCH("pay",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C35">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>2</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4144,7 +4143,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C1" t="s">
         <v>234</v>
@@ -4165,7 +4164,7 @@
         <v>239</v>
       </c>
       <c r="I1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4188,7 +4187,7 @@
         <v>292</v>
       </c>
       <c r="I2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4211,7 +4210,7 @@
         <v>292</v>
       </c>
       <c r="I3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4234,7 +4233,7 @@
         <v>292</v>
       </c>
       <c r="I4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -4257,7 +4256,7 @@
         <v>292</v>
       </c>
       <c r="I5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4274,18 +4273,18 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G6" t="s">
         <v>292</v>
       </c>
       <c r="I6" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -4297,13 +4296,13 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G7" t="s">
         <v>292</v>
       </c>
       <c r="I7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4418,7 +4417,7 @@
         <v>143</v>
       </c>
       <c r="I12" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -5178,13 +5177,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:I49">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$G2="yellow"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$G2="green"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$G2="red"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5910,7 +5909,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -5918,7 +5917,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B2">
         <v>-2</v>
@@ -5926,7 +5925,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B3">
         <v>0.5</v>
@@ -5934,7 +5933,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5942,7 +5941,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5950,7 +5949,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5958,7 +5957,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -5966,12 +5965,12 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5979,7 +5978,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B10">
         <v>-3</v>
@@ -6008,16 +6007,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D1" t="s">
         <v>327</v>
       </c>
-      <c r="D1" t="s">
-        <v>328</v>
-      </c>
       <c r="E1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6025,13 +6024,13 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D2" t="s">
+        <v>752</v>
+      </c>
+      <c r="E2" t="s">
         <v>753</v>
-      </c>
-      <c r="E2" t="s">
-        <v>754</v>
       </c>
       <c r="G2" t="s">
         <v>295</v>
@@ -6042,13 +6041,13 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D3" t="s">
+        <v>754</v>
+      </c>
+      <c r="E3" t="s">
         <v>755</v>
-      </c>
-      <c r="E3" t="s">
-        <v>756</v>
       </c>
       <c r="G3" t="s">
         <v>107</v>
@@ -6059,13 +6058,13 @@
         <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D4" t="s">
         <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G4" t="s">
         <v>296</v>
@@ -6076,7 +6075,7 @@
         <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
@@ -6090,7 +6089,7 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D6" t="s">
         <v>69</v>
@@ -6104,7 +6103,7 @@
         <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D7" t="s">
         <v>87</v>
@@ -6118,7 +6117,7 @@
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D8" t="s">
         <v>70</v>
@@ -6129,7 +6128,7 @@
         <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D9" t="s">
         <v>92</v>
@@ -6140,7 +6139,7 @@
         <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D10" t="s">
         <v>54</v>
@@ -6151,7 +6150,7 @@
         <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D11" t="s">
         <v>85</v>
@@ -6162,7 +6161,7 @@
         <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D12" t="s">
         <v>90</v>
@@ -6173,7 +6172,7 @@
         <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D13" t="s">
         <v>64</v>
@@ -6184,7 +6183,7 @@
         <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D14" t="s">
         <v>79</v>
@@ -6195,7 +6194,7 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D15" t="s">
         <v>79</v>
@@ -6206,7 +6205,7 @@
         <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D16" t="s">
         <v>79</v>
@@ -6217,7 +6216,7 @@
         <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D17" t="s">
         <v>43</v>
@@ -6228,7 +6227,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D18" t="s">
         <v>81</v>
@@ -6239,7 +6238,7 @@
         <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D19" t="s">
         <v>62</v>
@@ -6250,7 +6249,7 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D20" t="s">
         <v>34</v>
@@ -6261,7 +6260,7 @@
         <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D21" t="s">
         <v>76</v>
@@ -6272,7 +6271,7 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D22" t="s">
         <v>45</v>
@@ -6283,7 +6282,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D23" t="s">
         <v>56</v>
@@ -6294,7 +6293,7 @@
         <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D24" t="s">
         <v>36</v>
@@ -6305,7 +6304,7 @@
         <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
@@ -6316,7 +6315,7 @@
         <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D26" t="s">
         <v>101</v>
@@ -6327,7 +6326,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D27" t="s">
         <v>49</v>
@@ -6338,7 +6337,7 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D28" t="s">
         <v>51</v>
@@ -6349,7 +6348,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D29" t="s">
         <v>3</v>
@@ -6360,7 +6359,7 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
@@ -6371,7 +6370,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
@@ -6382,7 +6381,7 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -6393,7 +6392,7 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D33" t="s">
         <v>21</v>
@@ -6404,7 +6403,7 @@
         <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
@@ -6415,7 +6414,7 @@
         <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D35" t="s">
         <v>19</v>
@@ -6433,2103 +6432,2103 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
+        <v>329</v>
+      </c>
+      <c r="E38" t="s">
         <v>330</v>
-      </c>
-      <c r="E38" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="58" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="59" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="60" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="61" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="62" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="63" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="64" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="65" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="66" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="67" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="68" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="69" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="70" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="71" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="72" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="73" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="75" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="76" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="77" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="78" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="79" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="80" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="81" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="82" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="83" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="84" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D84" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="85" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="86" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="87" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="88" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="89" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D89" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="90" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D90" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="91" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D91" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="92" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="93" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D93" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="94" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D94" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="95" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D95" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="96" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D96" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="97" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="98" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D98" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="99" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="100" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D100" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="101" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="102" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="103" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="104" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="105" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D105" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="106" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="107" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="108" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="109" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="110" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="111" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="112" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D112" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="113" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="114" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="115" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="116" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D116" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="117" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="118" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="119" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="120" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="121" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D121" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="122" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D122" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="123" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="124" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="125" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="126" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="127" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="128" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="129" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="130" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D130" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="131" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="132" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="133" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="134" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D134" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="135" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D135" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="136" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D136" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="137" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="138" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="139" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="140" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="141" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="142" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="143" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="144" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="145" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="146" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D146" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="147" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
+        <v>439</v>
+      </c>
+      <c r="E147" t="s">
         <v>440</v>
-      </c>
-      <c r="E147" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="148" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="149" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="150" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="151" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="152" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="153" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="154" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="155" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="156" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="157" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="158" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="159" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D159" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="160" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D160" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="161" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D161" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="162" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="163" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="164" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="165" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D165" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="166" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D166" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="167" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="168" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="169" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D169" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="170" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D170" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="171" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="172" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D172" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D173" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="174" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D174" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="175" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D175" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="176" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D176" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="177" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D177" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="178" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D178" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="179" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D179" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="180" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="181" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="182" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D182" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="183" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D183" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="184" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D184" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="185" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D185" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="186" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D186" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="187" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="188" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="189" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D189" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="190" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D190" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="191" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D191" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="192" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D192" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="193" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D193" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="194" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D194" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="195" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="196" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D196" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="197" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D197" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="198" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D198" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="199" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D199" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="200" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="201" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="202" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D202" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="203" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D203" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="204" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D204" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="205" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D205" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="206" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D206" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="207" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D207" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="208" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D208" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="209" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D209" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="210" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D210" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="211" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D211" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="212" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D212" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="213" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D213" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="214" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D214" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="215" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="216" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D216" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="217" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D217" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="218" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D218" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="219" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D219" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="220" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D220" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="221" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D221" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="222" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D222" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="223" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D223" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="224" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D224" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="225" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D225" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="226" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D226" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="227" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D227" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="228" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D228" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="229" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D229" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="230" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D230" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="231" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D231" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="232" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D232" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="233" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D233" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="234" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D234" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="235" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D235" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="236" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D236" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="237" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D237" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="238" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D238" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="239" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D239" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="240" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D240" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="241" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D241" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="242" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D242" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="243" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D243" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="244" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D244" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="245" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D245" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="246" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D246" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="247" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D247" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="248" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D248" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="249" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D249" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="250" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D250" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="251" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D251" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="252" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D252" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="253" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D253" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="254" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D254" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="255" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D255" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="256" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D256" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="257" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D257" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="258" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D258" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="259" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D259" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="260" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D260" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="261" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D261" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="262" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D262" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="263" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D263" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="264" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D264" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="265" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D265" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="266" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D266" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="267" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D267" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="268" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D268" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="269" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D269" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="270" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D270" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="271" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D271" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="272" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D272" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="273" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D273" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="274" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D274" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="275" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D275" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="276" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D276" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="277" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D277" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="278" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D278" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="279" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D279" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="280" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D280" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="281" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D281" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="282" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D282" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="283" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D283" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="284" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D284" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="285" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D285" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="286" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D286" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="287" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D287" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="288" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D288" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="289" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D289" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="290" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D290" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="291" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D291" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="292" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D292" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="293" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D293" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="294" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D294" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="295" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D295" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="296" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D296" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="297" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D297" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="298" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D298" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="299" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D299" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="300" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D300" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="301" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D301" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="302" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D302" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="303" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D303" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="304" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D304" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="305" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D305" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="306" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D306" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="307" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D307" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="308" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D308" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="309" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D309" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="310" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D310" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="311" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D311" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="312" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D312" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="313" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D313" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="314" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D314" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="315" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D315" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="316" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D316" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="317" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D317" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="318" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D318" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="319" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D319" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="320" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D320" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="321" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D321" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="322" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D322" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="323" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D323" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="324" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D324" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="325" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D325" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="326" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D326" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="327" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D327" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="328" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D328" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="329" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D329" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="330" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D330" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="331" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D331" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="332" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D332" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="333" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D333" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="334" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D334" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="335" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D335" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="336" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D336" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="337" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D337" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="338" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D338" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="339" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D339" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="340" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D340" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="341" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D341" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="342" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D342" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="343" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D343" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="344" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D344" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="345" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D345" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="346" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D346" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="347" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D347" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="348" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D348" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="349" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D349" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="350" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D350" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="351" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D351" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="352" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D352" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="353" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D353" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="354" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D354" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="355" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D355" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="356" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D356" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="357" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D357" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="358" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D358" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="359" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D359" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="360" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D360" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="361" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D361" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="362" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D362" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="363" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D363" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="364" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D364" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="365" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D365" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="366" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D366" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="367" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D367" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="368" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D368" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="369" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D369" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="370" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D370" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="371" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D371" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="372" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D372" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="373" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D373" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="374" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D374" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="375" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D375" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="376" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D376" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="377" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D377" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="378" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D378" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="379" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D379" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="380" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D380" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="381" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D381" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="382" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D382" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="383" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D383" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="384" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D384" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="385" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D385" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="386" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D386" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="387" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D387" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="388" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D388" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="389" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D389" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="390" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D390" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="391" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D391" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="392" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D392" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="393" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D393" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="394" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D394" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="395" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D395" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="396" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D396" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="397" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D397" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="398" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D398" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="399" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D399" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="400" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D400" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="401" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D401" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="402" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D402" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="403" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D403" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="404" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D404" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="405" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D405" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="406" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D406" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="407" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D407" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="408" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D408" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="409" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D409" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="410" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D410" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="411" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D411" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="412" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D412" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="413" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D413" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="414" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D414" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="415" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D415" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="416" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D416" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="417" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D417" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="418" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D418" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="419" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D419" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="420" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D420" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="421" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D421" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="422" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D422" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="423" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D423" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="424" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D424" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="425" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D425" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="426" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D426" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="427" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D427" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="428" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D428" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="429" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D429" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="430" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D430" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="431" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D431" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="432" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D432" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="433" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D433" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="434" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D434" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="435" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D435" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="436" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D436" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="437" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D437" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="438" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D438" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="439" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D439" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="440" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D440" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="441" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D441" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="442" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D442" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="443" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D443" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="444" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D444" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="445" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D445" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="446" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D446" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="447" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D447" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="448" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D448" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="449" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D449" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="450" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D450" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="451" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D451" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="452" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D452" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="453" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D453" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="454" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D454" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="455" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D455" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="456" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D456" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add missing card to details
</commit_message>
<xml_diff>
--- a/Resources/details.xlsx
+++ b/Resources/details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alastair\OneDrive\Documents\Creative\Programming\Python\Caverna\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alastairc\Documents\Creative\Caverna\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="114_{6EE0B46E-ECCF-4B67-8489-EDE125484DF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{FBDFB1F9-B7F0-4B1E-8E5F-65AF2EB21900}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5883C393-A76E-48C5-9D44-4DBFDA380DB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{985A88D9-ACD6-4D50-8968-6DB430F624CA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{985A88D9-ACD6-4D50-8968-6DB430F624CA}"/>
   </bookViews>
   <sheets>
     <sheet name="action cards" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="773">
   <si>
     <t>name</t>
   </si>
@@ -2349,6 +2349,15 @@
   </si>
   <si>
     <t>twin tiles may overhang the edge and receive 2 coin per each overhanging tile</t>
+  </si>
+  <si>
+    <t>ruby mining 2</t>
+  </si>
+  <si>
+    <t>if player has at least 1 ruby mine then receive 1 ruby</t>
+  </si>
+  <si>
+    <t>always 1 ruby</t>
   </si>
 </sst>
 </file>
@@ -2462,11 +2471,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2480,145 +2489,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0C1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDDFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0C1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDDFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0C1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2646,20 +2517,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDDFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFE0C1FF"/>
         </patternFill>
       </fill>
@@ -2668,6 +2525,26 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2758,27 +2635,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2801,10 +2657,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D9CC4E6-CB70-411E-A7A4-573F16AAC537}" name="Table1" displayName="Table1" ref="A1:J35" totalsRowShown="0">
-  <autoFilter ref="A1:J35" xr:uid="{3766C5D4-C361-44B4-AD98-BAD8BD214D0C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I35">
-    <sortCondition ref="C1:C35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D9CC4E6-CB70-411E-A7A4-573F16AAC537}" name="Table1" displayName="Table1" ref="A1:J36" totalsRowShown="0">
+  <autoFilter ref="A1:J36" xr:uid="{3766C5D4-C361-44B4-AD98-BAD8BD214D0C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J36">
+    <sortCondition ref="C1:C36"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{C63C2947-CB53-4FED-8AA1-F4692B2F0544}" name="name"/>
@@ -2842,11 +2698,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A3CC4776-1BB1-47A4-A2A9-F8775571405D}" name="Table3" displayName="Table3" ref="A1:B53" totalsRowShown="0" dataDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A3CC4776-1BB1-47A4-A2A9-F8775571405D}" name="Table3" displayName="Table3" ref="A1:B53" totalsRowShown="0" dataDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A1:B53" xr:uid="{A4EB2E2A-BCC8-4327-8FD8-7B69602999D4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{59D50046-B7D9-4882-AFEC-FF0243C53E0B}" name="action value function output" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{13ED629A-1E3C-4AD1-844A-C53BC838B743}" name="value" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{59D50046-B7D9-4882-AFEC-FF0243C53E0B}" name="action value function output" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{13ED629A-1E3C-4AD1-844A-C53BC838B743}" name="value" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3160,10 +3016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15391F36-646A-4811-8FB5-C926ED9F13BD}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,75 +3455,72 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>-1</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>771</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
+        <v>772</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>-1</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="1">
-        <v>5</v>
-      </c>
-      <c r="J18" t="b">
-        <v>0</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>-1</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>75</v>
+        <v>35</v>
+      </c>
+      <c r="H19" s="1">
+        <v>5</v>
       </c>
       <c r="J19" t="b">
         <v>0</v>
@@ -3675,77 +3528,80 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>-1</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>32</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="1">
-        <v>5</v>
+        <v>77</v>
+      </c>
+      <c r="G20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="J20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>-1</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
       </c>
-      <c r="G21" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>75</v>
+      <c r="H21" s="1">
+        <v>5</v>
       </c>
       <c r="J21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>-1</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="1">
-        <v>5</v>
+      <c r="G22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="J22" t="b">
         <v>0</v>
@@ -3753,25 +3609,25 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>280</v>
+        <v>15</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
@@ -3779,19 +3635,19 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F24" t="s">
         <v>18</v>
@@ -3805,26 +3661,23 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F25" t="s">
         <v>18</v>
       </c>
-      <c r="G25" t="s">
-        <v>66</v>
-      </c>
       <c r="H25" s="1" t="s">
         <v>280</v>
       </c>
@@ -3834,13 +3687,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>321</v>
+        <v>49</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
         <v>68</v>
@@ -3852,9 +3705,9 @@
         <v>18</v>
       </c>
       <c r="G26" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>280</v>
       </c>
       <c r="J26" t="b">
@@ -3863,42 +3716,48 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>321</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>280</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="F28" t="s">
         <v>7</v>
@@ -3906,25 +3765,22 @@
       <c r="H28" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I28" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
@@ -3933,70 +3789,73 @@
         <v>280</v>
       </c>
       <c r="I29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>38</v>
+        <v>280</v>
+      </c>
+      <c r="I30" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>280</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>63</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>280</v>
@@ -4004,22 +3863,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F33" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="G33" t="s">
+        <v>30</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>280</v>
@@ -4027,19 +3886,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>97</v>
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
       </c>
       <c r="F34" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>280</v>
@@ -4047,185 +3909,205 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" t="s">
-        <v>317</v>
+        <v>15</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>24</v>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>770</v>
+      </c>
+      <c r="B36">
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" t="s">
+        <v>317</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38">
-        <f>COUNTIF(Table1[[action1]:[action2]], "take accumulated items")</f>
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
-      </c>
-      <c r="E39" t="s">
-        <v>104</v>
+        <v>28</v>
+      </c>
+      <c r="E39">
+        <f>COUNTIF(Table1[[action1]:[action2]], "take accumulated items")</f>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>103</v>
+        <v>47</v>
+      </c>
+      <c r="E40" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="D41" t="s">
-        <v>106</v>
-      </c>
-      <c r="E41" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E42" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D43" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E43" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>301</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>302</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>106</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>0</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>293</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C52">
         <v>5</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>296</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>297</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>298</v>
-      </c>
-      <c r="D54">
-        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
+        <v>298</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>299</v>
       </c>
-      <c r="D55">
+      <c r="D56">
         <v>5</v>
       </c>
     </row>
@@ -4233,26 +4115,26 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I31">
     <sortCondition ref="C31"/>
   </sortState>
-  <conditionalFormatting sqref="D2:E35">
-    <cfRule type="containsText" dxfId="6" priority="3" stopIfTrue="1" operator="containsText" text="take accumulated">
+  <conditionalFormatting sqref="D2:E36">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="furnish">
+      <formula>NOT(ISERROR(SEARCH("furnish",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="2" stopIfTrue="1" operator="containsText" text="baby dwarf">
+      <formula>NOT(ISERROR(SEARCH("baby dwarf",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="3" stopIfTrue="1" operator="containsText" text="take accumulated">
       <formula>NOT(ISERROR(SEARCH("take accumulated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="expedition">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="expedition">
       <formula>NOT(ISERROR(SEARCH("expedition",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" stopIfTrue="1" operator="containsText" text="baby dwarf">
-      <formula>NOT(ISERROR(SEARCH("baby dwarf",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="furnish">
-      <formula>NOT(ISERROR(SEARCH("furnish",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="place a">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="place a">
       <formula>NOT(ISERROR(SEARCH("place a",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="receive">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="receive">
       <formula>NOT(ISERROR(SEARCH("receive",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="pay">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="pay">
       <formula>NOT(ISERROR(SEARCH("pay",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5551,13 +5433,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:I49">
-    <cfRule type="expression" dxfId="34" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$G2="yellow"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$G2="green"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$G2="red"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>